<commit_message>
dynamic excel team export
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/egyeni_template.xlsx
+++ b/src/main/resources/templates/egyeni_template.xlsx
@@ -28,23 +28,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
-          <t>Szerző:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:area(lastCell = "K10")</t>
+          <t>jx:area(lastCell = "K10")</t>
         </r>
       </text>
     </comment>
@@ -52,23 +42,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
-          <t>Szerző:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="results" var="result" lastCell="k10")</t>
+          <t>jx:each(items="results" var="result" lastCell="k10")</t>
         </r>
       </text>
     </comment>
@@ -76,49 +56,42 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Szerző:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="result.individualCategory.contestants" var="contestant" lastCell="d5")</t>
+          <t>jx:each(items="result.individualCategory.contestants" var="contestant" lastCell="d5")</t>
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Szerző:</t>
+          <t>jx:each-merge(items="result.teamCategory.teams" var="team" lastCell="J5")</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0">
+      <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
-          <t xml:space="preserve">
-jx:each(items="result.teamCategory.teams" var="team" lastCell="K8")</t>
+          <t xml:space="preserve">jx:each(items="team.members" var="member" lastCell="I5")
+</t>
         </r>
       </text>
     </comment>
@@ -127,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Helyezés</t>
   </si>
@@ -165,45 +138,9 @@
     <t>${team.points}</t>
   </si>
   <si>
-    <t>${team.getMembers().get(0).getPosition()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(0).getNumber()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(0).getName()}</t>
-  </si>
-  <si>
     <t>${team.getMembers().get(0).getSchool().getName()}</t>
   </si>
   <si>
-    <t>${team.getMembers().get(1).getPosition()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(1).getNumber()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(1).getName()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(2).getPosition()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(2).getNumber()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(2).getName()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(3).getPosition()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(3).getNumber()}</t>
-  </si>
-  <si>
-    <t>${team.getMembers().get(3).getName()}</t>
-  </si>
-  <si>
     <t>${status.index = status.index +1}</t>
   </si>
   <si>
@@ -211,13 +148,22 @@
   </si>
   <si>
     <t>${contestant.position}</t>
+  </si>
+  <si>
+    <t>${member.position}</t>
+  </si>
+  <si>
+    <t>${member.number}</t>
+  </si>
+  <si>
+    <t>${member.name}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,22 +188,8 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -274,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -283,22 +215,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -316,7 +248,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -328,6 +260,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -337,149 +295,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -573,84 +388,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -988,19 +776,19 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="36.5703125" customWidth="1"/>
     <col min="11" max="11" width="36.7109375" customWidth="1"/>
   </cols>
@@ -1008,25 +796,25 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="F2" t="s">
-        <v>26</v>
+      <c r="E2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="F3" s="24" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1041,114 +829,96 @@
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="F4" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="33" t="s">
+      <c r="E5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>12</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="31"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="28"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="31"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="29"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="32"/>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="17"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -1162,12 +932,9 @@
       <c r="A15" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="E3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>